<commit_message>
athletics converted to excell
</commit_message>
<xml_diff>
--- a/athletics.xlsx
+++ b/athletics.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_F25DC773A252ABEACE02ECA09B5A67645ADE589E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{52297826-99D6-4A41-9BB6-697189E39DDD}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="11_F25DC773A252ABEACE02ECA09B5A67645ADE589E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{908E0A07-3B17-4CDB-B70F-C8501B655F42}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>page header</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Assistant Athletic Director: Open</t>
   </si>
   <si>
-    <t>Semi Finals:</t>
-  </si>
-  <si>
     <t>ScoreVision:</t>
   </si>
   <si>
@@ -62,6 +59,24 @@
   </si>
   <si>
     <t xml:space="preserve">Complete the online coaching application. Save it as a pdf and email it or print and mail the application to the Athletic Director at the address on form. Thank you. </t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>FBI Service Code is IKG6NX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In compliance with State regulations, York County School of Technology completes the Interscholastic Athletic Opportunities Disclosure Form in late October of each school year. This reporting requirement provides a detailed review of athletic programs offered by York County School of Technology and includes the number of students participating and the cost of each competitive athletic program for grades 9 through 12. </t>
+  </si>
+  <si>
+    <t>A copy of the report is available for review in the Administration Office.</t>
+  </si>
+  <si>
+    <t>Special Announcements:</t>
+  </si>
+  <si>
+    <t>Interscholastic Athletic Opportunities Discosure Form:</t>
   </si>
 </sst>
 </file>
@@ -379,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,37 +431,97 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>